<commit_message>
Création de grille aléatoire de jeu
</commit_message>
<xml_diff>
--- a/doc/Journal de Bord.xlsx
+++ b/doc/Journal de Bord.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CPNV\MA-20\Bataille-Navale\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{63A677C0-2549-43EF-881D-AB683B00F7D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13F3CDE-64E9-4855-AF9B-5E620530E210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4068" yWindow="132" windowWidth="18264" windowHeight="11712"/>
+    <workbookView xWindow="4068" yWindow="132" windowWidth="18264" windowHeight="11712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,16 +33,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>$</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Evénement</t>
+  </si>
+  <si>
+    <t>Fermeture des écoles et début du confinement</t>
+  </si>
+  <si>
+    <t>Découverte des gestions de fichiers sur C, comment les écrire, lire ainsi qu'append.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,16 +59,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -67,12 +97,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,19 +468,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="64.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D1" t="s">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>43903</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>43908</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Rendu final de la bataille navale version 1.0
</commit_message>
<xml_diff>
--- a/doc/Journal de Bord.xlsx
+++ b/doc/Journal de Bord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CPNV\MA-20\Bataille-Navale\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13F3CDE-64E9-4855-AF9B-5E620530E210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B8B1E3-2464-4DC4-ABA2-CF57FD25AD3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4068" yWindow="132" windowWidth="18264" windowHeight="11712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2208" yWindow="348" windowWidth="19224" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Découverte des gestions de fichiers sur C, comment les écrire, lire ainsi qu'append.</t>
+  </si>
+  <si>
+    <t>Rendu de la version 1.0 de l'application Bataille Navale</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,8 +507,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>43929</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -527,5 +535,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>